<commit_message>
Atualizado autoaprop.xlsx para IPM_PLJ
</commit_message>
<xml_diff>
--- a/outputs/autoaprop.xlsx/autoapropxlsx/IPM_PLJ.XLSX
+++ b/outputs/autoaprop.xlsx/autoapropxlsx/IPM_PLJ.XLSX
@@ -130,43 +130,44 @@
     <t>Domingo</t>
   </si>
   <si>
+    <t>JORGE LUIZ C MELLO</t>
+  </si>
+  <si>
+    <t>JOAO CARLOS M. SANTOS </t>
+  </si>
+  <si>
+    <t>ANTONIO P DOS SANTOS</t>
+  </si>
+  <si>
+    <t>DEVANI CORREA </t>
+  </si>
+  <si>
     <t>JOSE CARLOS VILELA</t>
   </si>
   <si>
-    <t> </t>
+    <t>LUCIANO DA SILVA SILVEIRA</t>
   </si>
   <si>
-    <t> </t>
+    <t>1091</t>
   </si>
   <si>
-    <t> </t>
+    <t>1625</t>
   </si>
   <si>
-    <t> </t>
+    <t>2088</t>
   </si>
   <si>
-    <t> </t>
+    <t>2412</t>
   </si>
   <si>
     <t>2831</t>
   </si>
   <si>
-    <t> </t>
+    <t>3687</t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t>SETOR  IPM PLANEJAMENTO</t>
+    <t>SETOR  IPM
+PLANEJAMENTO</t>
   </si>
   <si>
     <t>IPM_PLJ</t>
@@ -3518,103 +3519,103 @@
       </c>
       <c r="M12" s="174" t="str">
         <f>G12</f>
-        <v>JOSE CARLOS VILELA</v>
+        <v>JORGE LUIZ C MELLO</v>
       </c>
       <c r="N12" s="161"/>
       <c r="O12" s="187" t="str">
         <f>H12</f>
-        <v> </v>
+        <v>JOAO CARLOS M. SANTOS </v>
       </c>
       <c r="P12" s="161" t="str">
         <f>I12</f>
-        <v> </v>
+        <v>ANTONIO P DOS SANTOS</v>
       </c>
       <c r="Q12" s="161" t="str">
         <f>J12</f>
-        <v> </v>
+        <v>DEVANI CORREA </v>
       </c>
       <c r="R12" s="161" t="str">
         <f>K12</f>
-        <v> </v>
+        <v>JOSE CARLOS VILELA</v>
       </c>
       <c r="S12" s="161" t="str">
         <f>L12</f>
-        <v> </v>
+        <v>LUCIANO DA SILVA SILVEIRA</v>
       </c>
       <c r="T12" s="189"/>
       <c r="U12" s="174" t="str">
         <f>G12</f>
-        <v>JOSE CARLOS VILELA</v>
+        <v>JORGE LUIZ C MELLO</v>
       </c>
       <c r="V12" s="161"/>
       <c r="W12" s="161"/>
       <c r="X12" s="161" t="str">
         <f>H12</f>
-        <v> </v>
+        <v>JOAO CARLOS M. SANTOS </v>
       </c>
       <c r="Y12" s="161" t="str">
         <f>I12</f>
-        <v> </v>
+        <v>ANTONIO P DOS SANTOS</v>
       </c>
       <c r="Z12" s="161" t="str">
         <f>J12</f>
-        <v> </v>
+        <v>DEVANI CORREA </v>
       </c>
       <c r="AA12" s="161" t="str">
         <f>K12</f>
-        <v> </v>
+        <v>JOSE CARLOS VILELA</v>
       </c>
       <c r="AB12" s="161" t="str">
         <f>L12</f>
-        <v> </v>
+        <v>LUCIANO DA SILVA SILVEIRA</v>
       </c>
       <c r="AC12" s="181" t="str">
         <f t="shared" ref="AC12:AH12" si="0">G12</f>
-        <v>JOSE CARLOS VILELA</v>
+        <v>JORGE LUIZ C MELLO</v>
       </c>
       <c r="AD12" s="183" t="str">
         <f t="shared" si="0"/>
-        <v> </v>
+        <v>JOAO CARLOS M. SANTOS </v>
       </c>
       <c r="AE12" s="161" t="str">
         <f t="shared" si="0"/>
-        <v> </v>
+        <v>ANTONIO P DOS SANTOS</v>
       </c>
       <c r="AF12" s="161" t="str">
         <f t="shared" si="0"/>
-        <v> </v>
+        <v>DEVANI CORREA </v>
       </c>
       <c r="AG12" s="161" t="str">
         <f t="shared" si="0"/>
-        <v> </v>
+        <v>JOSE CARLOS VILELA</v>
       </c>
       <c r="AH12" s="161" t="str">
         <f t="shared" si="0"/>
-        <v> </v>
+        <v>LUCIANO DA SILVA SILVEIRA</v>
       </c>
       <c r="AI12" s="185" t="str">
         <f t="shared" ref="AI12:AN12" si="1">G12</f>
-        <v>JOSE CARLOS VILELA</v>
+        <v>JORGE LUIZ C MELLO</v>
       </c>
       <c r="AJ12" s="183" t="str">
         <f t="shared" si="1"/>
-        <v> </v>
+        <v>JOAO CARLOS M. SANTOS </v>
       </c>
       <c r="AK12" s="161" t="str">
         <f t="shared" si="1"/>
-        <v> </v>
+        <v>ANTONIO P DOS SANTOS</v>
       </c>
       <c r="AL12" s="161" t="str">
         <f t="shared" si="1"/>
-        <v> </v>
+        <v>DEVANI CORREA </v>
       </c>
       <c r="AM12" s="161" t="str">
         <f t="shared" si="1"/>
-        <v> </v>
+        <v>JOSE CARLOS VILELA</v>
       </c>
       <c r="AN12" s="161" t="str">
         <f t="shared" si="1"/>
-        <v> </v>
+        <v>LUCIANO DA SILVA SILVEIRA</v>
       </c>
     </row>
     <row r="13" spans="1:40" s="100" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3898,103 +3899,103 @@
       </c>
       <c r="M19" s="191" t="str">
         <f>G19</f>
-        <v>2831</v>
+        <v>1091</v>
       </c>
       <c r="N19" s="172"/>
       <c r="O19" s="172" t="str">
         <f>H19</f>
-        <v> </v>
+        <v>1625</v>
       </c>
       <c r="P19" s="172" t="str">
         <f>I19</f>
-        <v> </v>
+        <v>2088</v>
       </c>
       <c r="Q19" s="172" t="str">
         <f>J19</f>
-        <v> </v>
+        <v>2412</v>
       </c>
       <c r="R19" s="172" t="str">
         <f>K19</f>
-        <v> </v>
+        <v>2831</v>
       </c>
       <c r="S19" s="172" t="str">
         <f>L19</f>
-        <v> </v>
+        <v>3687</v>
       </c>
       <c r="T19" s="209"/>
       <c r="U19" s="191" t="str">
         <f>G19</f>
-        <v>2831</v>
+        <v>1091</v>
       </c>
       <c r="V19" s="172"/>
       <c r="W19" s="172"/>
       <c r="X19" s="172" t="str">
         <f>H19</f>
-        <v> </v>
+        <v>1625</v>
       </c>
       <c r="Y19" s="172" t="str">
         <f>I19</f>
-        <v> </v>
+        <v>2088</v>
       </c>
       <c r="Z19" s="172" t="str">
         <f>J19</f>
-        <v> </v>
+        <v>2412</v>
       </c>
       <c r="AA19" s="172" t="str">
         <f>K19</f>
-        <v> </v>
+        <v>2831</v>
       </c>
       <c r="AB19" s="172" t="str">
         <f>L19</f>
-        <v> </v>
+        <v>3687</v>
       </c>
       <c r="AC19" s="207" t="str">
         <f t="shared" ref="AC19:AH19" si="2">G19</f>
-        <v>2831</v>
+        <v>1091</v>
       </c>
       <c r="AD19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v> </v>
+        <v>1625</v>
       </c>
       <c r="AE19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v> </v>
+        <v>2088</v>
       </c>
       <c r="AF19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v> </v>
+        <v>2412</v>
       </c>
       <c r="AG19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v> </v>
+        <v>2831</v>
       </c>
       <c r="AH19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v> </v>
+        <v>3687</v>
       </c>
       <c r="AI19" s="205" t="str">
         <f t="shared" ref="AI19:AN19" si="3">G19</f>
-        <v>2831</v>
+        <v>1091</v>
       </c>
       <c r="AJ19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v> </v>
+        <v>1625</v>
       </c>
       <c r="AK19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v> </v>
+        <v>2088</v>
       </c>
       <c r="AL19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v> </v>
+        <v>2412</v>
       </c>
       <c r="AM19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v> </v>
+        <v>2831</v>
       </c>
       <c r="AN19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v> </v>
+        <v>3687</v>
       </c>
     </row>
     <row r="20" spans="1:40" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6093,7 +6094,8 @@
     <row r="1" spans="1:40" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="110" t="str">
         <f>'Segunda a Sexta'!A1:E9</f>
-        <v>SETOR  IPM PLANEJAMENTO</v>
+        <v>SETOR  IPM
+PLANEJAMENTO</v>
       </c>
       <c r="B1" s="111"/>
       <c r="C1" s="111"/>
@@ -6603,52 +6605,52 @@
       <c r="F12" s="159"/>
       <c r="G12" s="174" t="str">
         <f>'Segunda a Sexta'!G12:G18</f>
-        <v>JOSE CARLOS VILELA</v>
+        <v>JORGE LUIZ C MELLO</v>
       </c>
       <c r="H12" s="161" t="str">
         <f>'Segunda a Sexta'!H12:H18</f>
-        <v> </v>
+        <v>JOAO CARLOS M. SANTOS </v>
       </c>
       <c r="I12" s="161" t="str">
         <f>'Segunda a Sexta'!I12:I18</f>
-        <v> </v>
+        <v>ANTONIO P DOS SANTOS</v>
       </c>
       <c r="J12" s="161" t="str">
         <f>'Segunda a Sexta'!J12:J18</f>
-        <v> </v>
+        <v>DEVANI CORREA </v>
       </c>
       <c r="K12" s="161" t="str">
         <f>'Segunda a Sexta'!K12:K18</f>
-        <v> </v>
+        <v>JOSE CARLOS VILELA</v>
       </c>
       <c r="L12" s="161" t="str">
         <f>'Segunda a Sexta'!L12:L18</f>
-        <v> </v>
+        <v>LUCIANO DA SILVA SILVEIRA</v>
       </c>
       <c r="M12" s="174" t="str">
         <f>'Segunda a Sexta'!G12:G18</f>
-        <v>JOSE CARLOS VILELA</v>
+        <v>JORGE LUIZ C MELLO</v>
       </c>
       <c r="N12" s="161"/>
       <c r="O12" s="187" t="str">
         <f>'Segunda a Sexta'!H12:H18</f>
-        <v> </v>
+        <v>JOAO CARLOS M. SANTOS </v>
       </c>
       <c r="P12" s="187" t="str">
         <f>'Segunda a Sexta'!I12:I18</f>
-        <v> </v>
+        <v>ANTONIO P DOS SANTOS</v>
       </c>
       <c r="Q12" s="187" t="str">
         <f>'Segunda a Sexta'!J12:J18</f>
-        <v> </v>
+        <v>DEVANI CORREA </v>
       </c>
       <c r="R12" s="187" t="str">
         <f>'Segunda a Sexta'!K12:K18</f>
-        <v> </v>
+        <v>JOSE CARLOS VILELA</v>
       </c>
       <c r="S12" s="161" t="str">
         <f>'Segunda a Sexta'!L12:L18</f>
-        <v> </v>
+        <v>LUCIANO DA SILVA SILVEIRA</v>
       </c>
       <c r="T12" s="189"/>
       <c r="U12" s="262"/>
@@ -6935,52 +6937,52 @@
       </c>
       <c r="G19" s="258" t="str">
         <f>'Segunda a Sexta'!G19:G20</f>
-        <v>2831</v>
+        <v>1091</v>
       </c>
       <c r="H19" s="168" t="str">
         <f>'Segunda a Sexta'!H19:H20</f>
-        <v> </v>
+        <v>1625</v>
       </c>
       <c r="I19" s="168" t="str">
         <f>'Segunda a Sexta'!I19:I20</f>
-        <v> </v>
+        <v>2088</v>
       </c>
       <c r="J19" s="170" t="str">
         <f>'Segunda a Sexta'!J19:J20</f>
-        <v> </v>
+        <v>2412</v>
       </c>
       <c r="K19" s="172" t="str">
         <f>'Segunda a Sexta'!K19:K20</f>
-        <v> </v>
+        <v>2831</v>
       </c>
       <c r="L19" s="172" t="str">
         <f>'Segunda a Sexta'!L19:L20</f>
-        <v> </v>
+        <v>3687</v>
       </c>
       <c r="M19" s="191" t="str">
         <f>'Segunda a Sexta'!G19:G20</f>
-        <v>2831</v>
+        <v>1091</v>
       </c>
       <c r="N19" s="172"/>
       <c r="O19" s="257" t="str">
         <f>'Segunda a Sexta'!H19:H20</f>
-        <v> </v>
+        <v>1625</v>
       </c>
       <c r="P19" s="257" t="str">
         <f>'Segunda a Sexta'!I19:I20</f>
-        <v> </v>
+        <v>2088</v>
       </c>
       <c r="Q19" s="257" t="str">
         <f>'Segunda a Sexta'!J19:J20</f>
-        <v> </v>
+        <v>2412</v>
       </c>
       <c r="R19" s="257" t="str">
         <f>'Segunda a Sexta'!K19:K20</f>
-        <v> </v>
+        <v>2831</v>
       </c>
       <c r="S19" s="172" t="str">
         <f>'Segunda a Sexta'!L19:L20</f>
-        <v> </v>
+        <v>3687</v>
       </c>
       <c r="T19" s="209"/>
       <c r="U19" s="262"/>

</xml_diff>